<commit_message>
Fred: Full Rectangle implementation
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{567D7354-53FF-4978-8F23-DE1098219C62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13395749-1B26-4F60-A776-FDF483C6C369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1710" yWindow="585" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Frode</t>
   </si>
   <si>
-    <t>Tetiana</t>
-  </si>
-  <si>
     <t>Manju</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Nils Chr.</t>
+  </si>
+  <si>
+    <t>Tanya</t>
   </si>
 </sst>
 </file>
@@ -98,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +108,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6CDFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD0B9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,17 +154,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD0B9"/>
+      <color rgb="FFE6CDFF"/>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -446,230 +508,358 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="15" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
         <v>4</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="D7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10">
         <v>6</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="E10" s="10">
+        <v>6</v>
+      </c>
+      <c r="G10" s="8">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B11" s="10">
+        <v>6</v>
+      </c>
+      <c r="F11" s="9">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5</v>
+      </c>
+      <c r="G12" s="10">
+        <v>6</v>
+      </c>
+      <c r="I12" s="8">
+        <v>4</v>
+      </c>
+      <c r="K12" s="6">
+        <v>2</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="8">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10">
+        <v>6</v>
+      </c>
+      <c r="H13" s="9">
+        <v>5</v>
+      </c>
+      <c r="J13" s="7">
+        <v>3</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5</v>
+      </c>
+      <c r="I14" s="10">
+        <v>6</v>
+      </c>
+      <c r="K14" s="8">
+        <v>4</v>
+      </c>
+      <c r="M14" s="6">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="O15" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4</v>
+      </c>
+      <c r="F15" s="10">
+        <v>6</v>
+      </c>
+      <c r="J15" s="9">
+        <v>5</v>
+      </c>
+      <c r="L15" s="7">
+        <v>3</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fred: Updated pair stairs and Notes
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13395749-1B26-4F60-A776-FDF483C6C369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B34680-E590-4082-97C7-91DF8507CAFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="585" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
+    <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,18 +108,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -176,12 +164,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -508,7 +490,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +586,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="4"/>
@@ -624,7 +606,7 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5">
@@ -646,10 +628,10 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>4</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>2</v>
       </c>
       <c r="F6" s="4"/>
@@ -667,10 +649,10 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>3</v>
       </c>
       <c r="F7" s="5">
@@ -690,13 +672,13 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>6</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>4</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>2</v>
       </c>
       <c r="H8" s="4"/>
@@ -712,10 +694,10 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>5</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>3</v>
       </c>
       <c r="H9" s="5">
@@ -733,13 +715,13 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>6</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>4</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>2</v>
       </c>
       <c r="J10" s="4"/>
@@ -753,13 +735,13 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <v>6</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>5</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>3</v>
       </c>
       <c r="J11" s="5">
@@ -775,16 +757,16 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>5</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="8">
         <v>6</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <v>4</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>2</v>
       </c>
       <c r="L12" s="4"/>
@@ -796,16 +778,16 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>4</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="8">
         <v>6</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>5</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <v>3</v>
       </c>
       <c r="L13" s="5">
@@ -819,19 +801,19 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>5</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <v>6</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="6">
         <v>4</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="5">
         <v>2</v>
       </c>
       <c r="N14" s="4"/>
@@ -841,19 +823,19 @@
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <v>6</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <v>5</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="5">
         <v>3</v>
       </c>
       <c r="N15" s="5">

</xml_diff>

<commit_message>
Fred: Setting up more pairs in pairing stairs
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B34680-E590-4082-97C7-91DF8507CAFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBBC956-B520-439F-8C5B-7511240BF69D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -98,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +129,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -142,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -166,6 +178,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -174,6 +192,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF9B"/>
       <color rgb="FFFFD0B9"/>
       <color rgb="FFE6CDFF"/>
       <color rgb="FFCC99FF"/>
@@ -490,7 +509,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,6 +605,9 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
       <c r="C4" s="5">
         <v>2</v>
       </c>
@@ -652,6 +674,9 @@
       <c r="B7" s="7">
         <v>5</v>
       </c>
+      <c r="C7" s="10">
+        <v>8</v>
+      </c>
       <c r="D7" s="5">
         <v>3</v>
       </c>
@@ -678,6 +703,9 @@
       <c r="E8" s="6">
         <v>4</v>
       </c>
+      <c r="F8" s="10">
+        <v>8</v>
+      </c>
       <c r="G8" s="5">
         <v>2</v>
       </c>
@@ -694,6 +722,9 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
       <c r="D9" s="7">
         <v>5</v>
       </c>
@@ -715,6 +746,12 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C10" s="9">
+        <v>7</v>
+      </c>
+      <c r="D10" s="10">
+        <v>8</v>
+      </c>
       <c r="E10" s="8">
         <v>6</v>
       </c>
@@ -738,8 +775,14 @@
       <c r="B11" s="8">
         <v>6</v>
       </c>
+      <c r="D11" s="9">
+        <v>7</v>
+      </c>
       <c r="F11" s="7">
         <v>5</v>
+      </c>
+      <c r="G11" s="10">
+        <v>8</v>
       </c>
       <c r="H11" s="5">
         <v>3</v>
@@ -760,11 +803,17 @@
       <c r="C12" s="7">
         <v>5</v>
       </c>
+      <c r="E12" s="9">
+        <v>7</v>
+      </c>
       <c r="G12" s="8">
         <v>6</v>
       </c>
       <c r="I12" s="6">
         <v>4</v>
+      </c>
+      <c r="J12" s="10">
+        <v>8</v>
       </c>
       <c r="K12" s="5">
         <v>2</v>
@@ -784,6 +833,12 @@
       <c r="D13" s="8">
         <v>6</v>
       </c>
+      <c r="E13" s="10">
+        <v>8</v>
+      </c>
+      <c r="F13" s="9">
+        <v>7</v>
+      </c>
       <c r="H13" s="7">
         <v>5</v>
       </c>
@@ -807,6 +862,12 @@
       <c r="E14" s="7">
         <v>5</v>
       </c>
+      <c r="G14" s="9">
+        <v>7</v>
+      </c>
+      <c r="H14" s="10">
+        <v>8</v>
+      </c>
       <c r="I14" s="8">
         <v>6</v>
       </c>
@@ -831,6 +892,9 @@
       </c>
       <c r="F15" s="8">
         <v>6</v>
+      </c>
+      <c r="H15" s="9">
+        <v>7</v>
       </c>
       <c r="J15" s="7">
         <v>5</v>

</xml_diff>

<commit_message>
Fred: More updates to pair-stairs
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBBC956-B520-439F-8C5B-7511240BF69D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A5DA00-30DB-48B6-A6C9-95BE163FDF66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -113,12 +113,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE6CDFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -138,6 +132,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,7 +509,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +631,9 @@
       <c r="B5" s="5">
         <v>3</v>
       </c>
+      <c r="C5" s="10">
+        <v>9</v>
+      </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
@@ -650,7 +653,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="E6" s="5">
@@ -671,10 +674,10 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>8</v>
       </c>
       <c r="D7" s="5">
@@ -697,13 +700,16 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>6</v>
       </c>
-      <c r="E8" s="6">
+      <c r="D8" s="10">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5">
         <v>4</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>8</v>
       </c>
       <c r="G8" s="5">
@@ -722,14 +728,17 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>7</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>5</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
+      </c>
+      <c r="G9" s="10">
+        <v>9</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -746,16 +755,16 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>7</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>6</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>4</v>
       </c>
       <c r="I10" s="5">
@@ -772,16 +781,19 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>6</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>7</v>
       </c>
-      <c r="F11" s="7">
+      <c r="E11" s="10">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6">
         <v>5</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>8</v>
       </c>
       <c r="H11" s="5">
@@ -800,19 +812,22 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>7</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>6</v>
       </c>
-      <c r="I12" s="6">
+      <c r="H12" s="10">
+        <v>9</v>
+      </c>
+      <c r="I12" s="5">
         <v>4</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>8</v>
       </c>
       <c r="K12" s="5">
@@ -827,19 +842,19 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>6</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>8</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>7</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>5</v>
       </c>
       <c r="J13" s="5">
@@ -856,22 +871,28 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="B14" s="10">
+        <v>9</v>
+      </c>
       <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>5</v>
       </c>
-      <c r="G14" s="9">
+      <c r="F14" s="10">
+        <v>9</v>
+      </c>
+      <c r="G14" s="8">
         <v>7</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>8</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>6</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>4</v>
       </c>
       <c r="M14" s="5">
@@ -887,16 +908,19 @@
       <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>4</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>6</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>7</v>
       </c>
-      <c r="J15" s="7">
+      <c r="I15" s="10">
+        <v>9</v>
+      </c>
+      <c r="J15" s="6">
         <v>5</v>
       </c>
       <c r="L15" s="5">

</xml_diff>

<commit_message>
Fred: Quantity with temperature equality and hashCode()
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252E3BC5-98F2-44FA-9E1F-7C4E53D281B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1ED92F-321C-483D-9F93-14982E6F4316}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Thor Erik</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>6(7)</t>
+  </si>
+  <si>
+    <t>7(1)</t>
+  </si>
+  <si>
+    <t>7(2)</t>
+  </si>
+  <si>
+    <t>7(3)</t>
+  </si>
+  <si>
+    <t>7(4)</t>
+  </si>
+  <si>
+    <t>7(5)</t>
+  </si>
+  <si>
+    <t>7(6)</t>
+  </si>
+  <si>
+    <t>7(7)</t>
   </si>
 </sst>
 </file>
@@ -140,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,12 +171,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6CDFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -221,9 +236,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -551,7 +563,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +685,7 @@
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>9</v>
       </c>
       <c r="D5" s="5">
@@ -716,10 +728,10 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>8</v>
       </c>
       <c r="D7" s="5">
@@ -742,16 +754,16 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>9</v>
       </c>
       <c r="E8" s="5">
         <v>4</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>8</v>
       </c>
       <c r="G8" s="5">
@@ -770,16 +782,16 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>9</v>
       </c>
       <c r="H9" s="5">
@@ -797,13 +809,13 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8">
-        <v>7</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="C10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="8">
         <v>8</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="5">
@@ -823,19 +835,19 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="8">
-        <v>7</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="9">
         <v>9</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>8</v>
       </c>
       <c r="H11" s="5">
@@ -854,22 +866,22 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8">
-        <v>7</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <v>9</v>
       </c>
       <c r="I12" s="5">
         <v>4</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <v>8</v>
       </c>
       <c r="K12" s="5">
@@ -887,16 +899,16 @@
       <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>8</v>
       </c>
-      <c r="F13" s="8">
-        <v>7</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="F13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="5">
@@ -913,25 +925,25 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>9</v>
       </c>
       <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>9</v>
       </c>
-      <c r="G14" s="8">
-        <v>7</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="G14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="8">
         <v>8</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>27</v>
       </c>
       <c r="K14" s="5">
@@ -953,16 +965,16 @@
       <c r="D15" s="5">
         <v>4</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="8">
-        <v>7</v>
-      </c>
-      <c r="I15" s="10">
+      <c r="H15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="9">
         <v>9</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="5">

</xml_diff>

<commit_message>
Fred: Graph with canReach() using functional operator
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1ED92F-321C-483D-9F93-14982E6F4316}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF48516-AF20-439F-BFA0-F4C83C5D328C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Thor Erik</t>
   </si>
@@ -139,13 +139,31 @@
   </si>
   <si>
     <t>7(7)</t>
+  </si>
+  <si>
+    <t>8(1)</t>
+  </si>
+  <si>
+    <t>8(2)</t>
+  </si>
+  <si>
+    <t>8(3)</t>
+  </si>
+  <si>
+    <t>8(4)</t>
+  </si>
+  <si>
+    <t>8(5)</t>
+  </si>
+  <si>
+    <t>8(6)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +178,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +200,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD0B9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF9B"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -189,12 +207,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,9 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,12 +241,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF04234-83B0-40FE-A3F9-0E03A22D7DBB}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B1" sqref="B1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,10 +604,10 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -619,371 +627,356 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="9">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>4</v>
       </c>
-      <c r="F8" s="8">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
         <v>2</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="5">
+      <c r="E9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="9">
-        <v>9</v>
-      </c>
-      <c r="H9" s="5">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="8">
-        <v>8</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>4</v>
       </c>
-      <c r="I10" s="5">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
         <v>2</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="9">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="8">
-        <v>8</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
         <v>3</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>1</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="9">
-        <v>9</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
         <v>4</v>
       </c>
-      <c r="J12" s="8">
-        <v>8</v>
-      </c>
-      <c r="K12" s="5">
+      <c r="J12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="4">
         <v>2</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="8">
-        <v>8</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>3</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>1</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9">
-        <v>9</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4">
         <v>3</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="9">
-        <v>9</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="F14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="8">
-        <v>8</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="4">
         <v>4</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="4">
         <v>2</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="9">
-        <v>9</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="5">
+      <c r="K15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="4">
         <v>3</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="4">
         <v>1</v>
       </c>
-      <c r="O15" s="4"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fred: Graph with minimum hopCount(); used for loop; bug exists!
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF48516-AF20-439F-BFA0-F4C83C5D328C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE75F2B-49CE-4531-B150-144C35D6866F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -200,13 +200,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF9B"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,14 +238,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:O1"/>
+      <selection activeCell="O1" activeCellId="2" sqref="M15 M1 O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,46 +580,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -667,7 +667,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="4">
@@ -716,6 +716,9 @@
       <c r="C6" s="4">
         <v>4</v>
       </c>
+      <c r="D6" s="9">
+        <v>9</v>
+      </c>
       <c r="E6" s="4">
         <v>2</v>
       </c>
@@ -755,7 +758,7 @@
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -781,19 +784,21 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="9">
+        <v>9</v>
+      </c>
       <c r="H9" s="4">
         <v>1</v>
       </c>
@@ -809,7 +814,7 @@
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="4"/>
@@ -819,7 +824,9 @@
       <c r="G10" s="4">
         <v>4</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="9">
+        <v>9</v>
+      </c>
       <c r="I10" s="4">
         <v>2</v>
       </c>
@@ -837,10 +844,12 @@
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="9">
+        <v>9</v>
+      </c>
       <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
@@ -864,7 +873,7 @@
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -874,7 +883,7 @@
       <c r="I12" s="4">
         <v>4</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K12" s="4">
@@ -895,10 +904,10 @@
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -918,17 +927,19 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="9">
+        <v>9</v>
+      </c>
       <c r="C14" s="4">
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H14" s="4"/>
@@ -957,26 +968,29 @@
       <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="K15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L15" s="4">
         <v>3</v>
       </c>
+      <c r="M15" s="9">
+        <v>9</v>
+      </c>
       <c r="N15" s="4">
         <v>1</v>
       </c>
       <c r="O15" s="3"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fred: Graph with costs
</commit_message>
<xml_diff>
--- a/doc/pair_stairs.xlsx
+++ b/doc/pair_stairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\src\kotlin\oo_boot_camp_2021-05-03_kotlin\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE75F2B-49CE-4531-B150-144C35D6866F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599E2E55-56C7-4204-91D0-AC49DA35C0DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="585" yWindow="2280" windowWidth="15990" windowHeight="13020" xr2:uid="{CB6CA43E-D666-4DC3-91E9-F94436A359DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Thor Erik</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>8(6)</t>
+  </si>
+  <si>
+    <t>9(1)</t>
+  </si>
+  <si>
+    <t>9(2)</t>
+  </si>
+  <si>
+    <t>9(4)</t>
+  </si>
+  <si>
+    <t>9(3)</t>
+  </si>
+  <si>
+    <t>9(5)</t>
+  </si>
+  <si>
+    <t>9(6)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +228,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -223,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -246,6 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +596,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" activeCellId="2" sqref="M15 M1 O1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,8 +741,8 @@
       <c r="C6" s="4">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
-        <v>9</v>
+      <c r="D6" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -796,8 +821,8 @@
       <c r="F9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="9">
-        <v>9</v>
+      <c r="G9" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="H9" s="4">
         <v>1</v>
@@ -824,8 +849,8 @@
       <c r="G10" s="4">
         <v>4</v>
       </c>
-      <c r="H10" s="9">
-        <v>9</v>
+      <c r="H10" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
@@ -847,8 +872,8 @@
       <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="9">
-        <v>9</v>
+      <c r="E11" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>18</v>
@@ -867,7 +892,7 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -927,8 +952,8 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9">
-        <v>9</v>
+      <c r="B14" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="4">
         <v>3</v>
@@ -981,8 +1006,8 @@
       <c r="L15" s="4">
         <v>3</v>
       </c>
-      <c r="M15" s="9">
-        <v>9</v>
+      <c r="M15" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="N15" s="4">
         <v>1</v>

</xml_diff>